<commit_message>
Integrated multilanguage into recipe search as well
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople_v9.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople_v9.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9668" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9686" uniqueCount="1414">
   <si>
     <t>id</t>
   </si>
@@ -4223,6 +4223,57 @@
   </si>
   <si>
     <t>Verdure</t>
+  </si>
+  <si>
+    <t>vegetarian</t>
+  </si>
+  <si>
+    <t>vegan</t>
+  </si>
+  <si>
+    <t>onnivore</t>
+  </si>
+  <si>
+    <t>lactose</t>
+  </si>
+  <si>
+    <t>gluten</t>
+  </si>
+  <si>
+    <t>vegetariano</t>
+  </si>
+  <si>
+    <t>vegano</t>
+  </si>
+  <si>
+    <t>onnivoro</t>
+  </si>
+  <si>
+    <t>lattosio</t>
+  </si>
+  <si>
+    <t>glutine</t>
+  </si>
+  <si>
+    <t>Primo Seminario sui Meze</t>
+  </si>
+  <si>
+    <t>Secondo Seminario sui Meze</t>
+  </si>
+  <si>
+    <t>Terzo Seminario sui Meze</t>
+  </si>
+  <si>
+    <t>In the kitchen beyond borders</t>
+  </si>
+  <si>
+    <t>peperoncino piccante rosso</t>
+  </si>
+  <si>
+    <t>padellina</t>
+  </si>
+  <si>
+    <t>padella da frittura</t>
   </si>
 </sst>
 </file>
@@ -4813,9 +4864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G79"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9866,7 +9915,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10072,7 +10121,7 @@
   <dimension ref="A1:F896"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28314,7 +28363,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28409,8 +28458,8 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>457</v>
+      <c r="B5" s="4" t="s">
+        <v>1410</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>455</v>
@@ -29118,8 +29167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C179"/>
   <sheetViews>
-    <sheetView topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B126" sqref="B126:B177"/>
+    <sheetView topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31082,7 +31131,7 @@
   <dimension ref="A1:AMK241"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36650,10 +36699,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J529"/>
+  <dimension ref="A1:J538"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="B208" sqref="B208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40927,7 +40976,7 @@
         <v>419</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>1046</v>
+        <v>1413</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>1080</v>
@@ -44305,7 +44354,7 @@
         <v>162</v>
       </c>
       <c r="B378" s="4" t="s">
-        <v>976</v>
+        <v>1411</v>
       </c>
       <c r="C378" s="4" t="s">
         <v>784</v>
@@ -45173,7 +45222,7 @@
         <v>427</v>
       </c>
       <c r="B422" s="4" t="s">
-        <v>1046</v>
+        <v>1412</v>
       </c>
       <c r="C422" s="4" t="s">
         <v>1080</v>
@@ -47266,6 +47315,78 @@
       </c>
       <c r="D529" s="4" t="s">
         <v>698</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A530" s="4" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B530" s="4" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A531" s="4" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B531" s="4" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A532" s="4" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B532" s="4" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A533" s="4" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B533" s="4" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A534" s="4" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B534" s="4" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A535" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B535" s="4" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A536" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B536" s="4" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A537" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B537" s="4" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A538" s="4" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B538" s="4" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getter getEvetnsRecipes, and multilanguage for last getters
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople_v9.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople_v9.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9686" uniqueCount="1422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9690" uniqueCount="1425">
   <si>
     <t>id</t>
   </si>
@@ -4298,6 +4298,15 @@
   </si>
   <si>
     <t>asia/thailand/thai-chicken-in-green-curry</t>
+  </si>
+  <si>
+    <t>seminario</t>
+  </si>
+  <si>
+    <t>charity dinner</t>
+  </si>
+  <si>
+    <t>cena di beneficenza</t>
   </si>
 </sst>
 </file>
@@ -4888,7 +4897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -36762,10 +36771,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J538"/>
+  <dimension ref="A1:J540"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A529" workbookViewId="0">
+      <selection activeCell="A540" sqref="A540"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47450,6 +47459,22 @@
       </c>
       <c r="D538" s="4" t="s">
         <v>625</v>
+      </c>
+    </row>
+    <row r="539" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A539" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B539" s="4" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="540" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A540" s="4" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B540" s="4" t="s">
+        <v>1424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multilanguage support for all getters used by UI
</commit_message>
<xml_diff>
--- a/data_sources/scripts/files/FoodConnectsPeople_v9.xlsx
+++ b/data_sources/scripts/files/FoodConnectsPeople_v9.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" firstSheet="3" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="993" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Recipe" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10179" uniqueCount="1655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10179" uniqueCount="1656">
   <si>
     <t>id</t>
   </si>
@@ -4998,6 +4998,9 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>red chili</t>
   </si>
 </sst>
 </file>
@@ -5612,8 +5615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P79"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9095,7 +9098,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>1138</v>
+        <v>539</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>1296</v>
@@ -9432,7 +9435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -32124,7 +32127,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G241"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="A177" sqref="A177"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37683,8 +37688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J767"/>
   <sheetViews>
-    <sheetView topLeftCell="A529" workbookViewId="0">
-      <selection activeCell="A529" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="A383" sqref="A383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45337,7 +45342,7 @@
     </row>
     <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" s="4" t="s">
-        <v>398</v>
+        <v>1655</v>
       </c>
       <c r="B383" s="4" t="s">
         <v>901</v>

</xml_diff>